<commit_message>
Added a copy of the FRAP analysis Excel file and updated some plotting scripts.  Added a copy of notes on hydrogels.
</commit_message>
<xml_diff>
--- a/FRAP-results/FRAP-analysis-190605.xlsx
+++ b/FRAP-results/FRAP-analysis-190605.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauramaguire/Google Drive/Thesis/Thesis Repository/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauramaguire/Google Drive/Thesis/Thesis Repository/FRAP-results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AA6963-A156-4548-BC83-296741BE829B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308B8F0D-06D3-C442-AE5D-119B4D47963B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="6" xr2:uid="{A9073BF0-BA06-8246-BE23-0DC2BC3153F9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="5" xr2:uid="{A9073BF0-BA06-8246-BE23-0DC2BC3153F9}"/>
   </bookViews>
   <sheets>
     <sheet name="List of datasets" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="315">
   <si>
     <t>Gel type</t>
   </si>
@@ -1011,12 +1011,27 @@
   <si>
     <t>Value</t>
   </si>
+  <si>
+    <t>predicted off-rate (upper Nt bound)</t>
+  </si>
+  <si>
+    <t>s^-1</t>
+  </si>
+  <si>
+    <t>predicted off-rate upper Nt bound</t>
+  </si>
+  <si>
+    <t>experimental DB/DF</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1026,13 +1041,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1217,7 +1225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1288,7 +1296,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1343,13 +1350,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1403,6 +1409,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7477,510 +7492,510 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="104"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="61" t="s">
+      <c r="A1" s="102"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="60" t="s">
         <v>290</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="60" t="s">
         <v>290</v>
       </c>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
     </row>
     <row r="2" spans="1:8" ht="17">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="105" t="s">
         <v>239</v>
       </c>
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="92" t="s">
         <v>238</v>
       </c>
-      <c r="C2" s="94" t="s">
+      <c r="C2" s="92" t="s">
         <v>237</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="59" t="s">
         <v>236</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="59" t="s">
         <v>235</v>
       </c>
-      <c r="F2" s="98" t="s">
+      <c r="F2" s="96" t="s">
         <v>293</v>
       </c>
-      <c r="G2" s="98" t="s">
+      <c r="G2" s="96" t="s">
         <v>292</v>
       </c>
-      <c r="H2" s="60" t="s">
+      <c r="H2" s="59" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="108">
+      <c r="A3" s="106">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="54" t="s">
         <v>211</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="D3" s="63">
+      <c r="D3" s="62">
         <v>41.575180990369098</v>
       </c>
-      <c r="E3" s="63">
+      <c r="E3" s="62">
         <v>26.701718003743199</v>
       </c>
-      <c r="F3" s="63">
+      <c r="F3" s="62">
         <v>0.63847559224578498</v>
       </c>
-      <c r="G3" s="63">
+      <c r="G3" s="62">
         <v>0.51804560706973102</v>
       </c>
-      <c r="H3" s="63">
+      <c r="H3" s="62">
         <f t="shared" ref="H3:H16" si="0">1-G3/F3</f>
         <v>0.18862112606756265</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="104">
+      <c r="A4" s="102">
         <v>4</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="53" t="s">
         <v>210</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="53" t="s">
         <v>196</v>
       </c>
-      <c r="D4" s="58">
+      <c r="D4" s="57">
         <v>68.653690590885404</v>
       </c>
-      <c r="E4" s="58">
+      <c r="E4" s="57">
         <v>71.213773666190406</v>
       </c>
-      <c r="F4" s="58">
+      <c r="F4" s="57">
         <v>0.570302574906566</v>
       </c>
-      <c r="G4" s="58">
+      <c r="G4" s="57">
         <v>0.51505930004399503</v>
       </c>
-      <c r="H4" s="58">
+      <c r="H4" s="57">
         <f t="shared" si="0"/>
         <v>9.6866606067176897E-2</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="108">
+      <c r="A5" s="106">
         <v>7</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="D5" s="63">
+      <c r="D5" s="62">
         <v>25.2802362976125</v>
       </c>
-      <c r="E5" s="63">
+      <c r="E5" s="62">
         <v>26.402570800341099</v>
       </c>
-      <c r="F5" s="63">
+      <c r="F5" s="62">
         <v>0.51542088790752405</v>
       </c>
-      <c r="G5" s="63">
+      <c r="G5" s="62">
         <v>0.52152694410839195</v>
       </c>
-      <c r="H5" s="63">
+      <c r="H5" s="62">
         <f t="shared" si="0"/>
         <v>-1.1846737965271359E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="104">
+      <c r="A6" s="102">
         <v>13</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="53" t="s">
         <v>207</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="53" t="s">
         <v>196</v>
       </c>
-      <c r="D6" s="58">
+      <c r="D6" s="57">
         <v>71.993960006430498</v>
       </c>
-      <c r="E6" s="58">
+      <c r="E6" s="57">
         <v>71.499631169558</v>
       </c>
-      <c r="F6" s="58">
+      <c r="F6" s="57">
         <v>0.65976374422412598</v>
       </c>
-      <c r="G6" s="58">
+      <c r="G6" s="57">
         <v>0.61288586158568203</v>
       </c>
-      <c r="H6" s="58">
+      <c r="H6" s="57">
         <f t="shared" si="0"/>
         <v>7.1052529104295936E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="108">
+      <c r="A7" s="106">
         <v>18</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="54" t="s">
         <v>206</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="D7" s="63">
+      <c r="D7" s="62">
         <v>33.133739311413898</v>
       </c>
-      <c r="E7" s="63">
+      <c r="E7" s="62">
         <v>25.8287038913023</v>
       </c>
-      <c r="F7" s="63">
+      <c r="F7" s="62">
         <v>0.43777082911985499</v>
       </c>
-      <c r="G7" s="63">
+      <c r="G7" s="62">
         <v>0.472163938441783</v>
       </c>
-      <c r="H7" s="63">
+      <c r="H7" s="62">
         <f t="shared" si="0"/>
         <v>-7.8564187090939486E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="104">
+      <c r="A8" s="102">
         <v>20</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="53" t="s">
         <v>205</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="53" t="s">
         <v>196</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="57">
         <v>100.117458589465</v>
       </c>
-      <c r="E8" s="58">
+      <c r="E8" s="57">
         <v>68.139648991330205</v>
       </c>
-      <c r="F8" s="58">
+      <c r="F8" s="57">
         <v>0.42256801874060901</v>
       </c>
-      <c r="G8" s="58">
+      <c r="G8" s="57">
         <v>0.49165399158114997</v>
       </c>
-      <c r="H8" s="58">
+      <c r="H8" s="57">
         <f t="shared" si="0"/>
         <v>-0.16349077492054365</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="108">
+      <c r="A9" s="106">
         <v>24</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="54" t="s">
         <v>204</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="D9" s="63">
+      <c r="D9" s="62">
         <v>26.832919607273801</v>
       </c>
-      <c r="E9" s="63">
+      <c r="E9" s="62">
         <v>26.520995286782401</v>
       </c>
-      <c r="F9" s="63">
+      <c r="F9" s="62">
         <v>0.20572810225569299</v>
       </c>
-      <c r="G9" s="63">
+      <c r="G9" s="62">
         <v>0.29748988283993699</v>
       </c>
-      <c r="H9" s="63">
+      <c r="H9" s="62">
         <f t="shared" si="0"/>
         <v>-0.44603425384343542</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="104">
+      <c r="A10" s="102">
         <v>25</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="53" t="s">
         <v>203</v>
       </c>
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="53" t="s">
         <v>196</v>
       </c>
-      <c r="D10" s="58">
+      <c r="D10" s="57">
         <v>31.162829923525099</v>
       </c>
-      <c r="E10" s="58">
+      <c r="E10" s="57">
         <v>27.622707706662698</v>
       </c>
-      <c r="F10" s="58">
+      <c r="F10" s="57">
         <v>0.39634094192997399</v>
       </c>
-      <c r="G10" s="58">
+      <c r="G10" s="57">
         <v>0.41780485629553299</v>
       </c>
-      <c r="H10" s="58">
+      <c r="H10" s="57">
         <f t="shared" si="0"/>
         <v>-5.4155178269095661E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="108">
+      <c r="A11" s="106">
         <v>26</v>
       </c>
-      <c r="B11" s="109" t="s">
+      <c r="B11" s="107" t="s">
         <v>266</v>
       </c>
-      <c r="C11" s="55" t="s">
+      <c r="C11" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="D11" s="63">
+      <c r="D11" s="62">
         <v>74.782954302142599</v>
       </c>
-      <c r="E11" s="63">
+      <c r="E11" s="62">
         <v>61.437581286543498</v>
       </c>
-      <c r="F11" s="63">
+      <c r="F11" s="62">
         <v>0.48172188415206202</v>
       </c>
-      <c r="G11" s="63">
+      <c r="G11" s="62">
         <v>0.45080865072624798</v>
       </c>
-      <c r="H11" s="63">
+      <c r="H11" s="62">
         <f t="shared" si="0"/>
         <v>6.4172366759355781E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="104">
+      <c r="A12" s="102">
         <v>28</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="53" t="s">
         <v>201</v>
       </c>
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="53" t="s">
         <v>196</v>
       </c>
-      <c r="D12" s="58">
+      <c r="D12" s="57">
         <v>10.8688914113787</v>
       </c>
-      <c r="E12" s="58">
+      <c r="E12" s="57">
         <v>15.207550491225399</v>
       </c>
-      <c r="F12" s="58">
+      <c r="F12" s="57">
         <v>0.41937615905339198</v>
       </c>
-      <c r="G12" s="58">
+      <c r="G12" s="57">
         <v>0.42485405650164798</v>
       </c>
-      <c r="H12" s="58">
+      <c r="H12" s="57">
         <f t="shared" si="0"/>
         <v>-1.3062014446936221E-2</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="108">
+      <c r="A13" s="106">
         <v>30</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="54" t="s">
         <v>200</v>
       </c>
-      <c r="C13" s="55" t="s">
+      <c r="C13" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="D13" s="63">
+      <c r="D13" s="62">
         <v>37.793977203101903</v>
       </c>
-      <c r="E13" s="63">
+      <c r="E13" s="62">
         <v>31.9935373143629</v>
       </c>
-      <c r="F13" s="63">
+      <c r="F13" s="62">
         <v>0.528499139535201</v>
       </c>
-      <c r="G13" s="63">
+      <c r="G13" s="62">
         <v>0.52038476601907702</v>
       </c>
-      <c r="H13" s="63">
+      <c r="H13" s="62">
         <f t="shared" si="0"/>
         <v>1.5353617270333353E-2</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="104">
+      <c r="A14" s="102">
         <v>31</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="53" t="s">
         <v>199</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="53" t="s">
         <v>196</v>
       </c>
-      <c r="D14" s="58">
+      <c r="D14" s="57">
         <v>18.333919291963401</v>
       </c>
-      <c r="E14" s="58">
+      <c r="E14" s="57">
         <v>15.584490555396</v>
       </c>
-      <c r="F14" s="58">
+      <c r="F14" s="57">
         <v>0.39409600550881702</v>
       </c>
-      <c r="G14" s="58">
+      <c r="G14" s="57">
         <v>0.42347882825524402</v>
       </c>
-      <c r="H14" s="58">
+      <c r="H14" s="57">
         <f t="shared" si="0"/>
         <v>-7.4557524906883721E-2</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="108">
+      <c r="A15" s="106">
         <v>33</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="54" t="s">
         <v>198</v>
       </c>
-      <c r="C15" s="55" t="s">
+      <c r="C15" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="D15" s="63">
+      <c r="D15" s="62">
         <v>40.789211507413903</v>
       </c>
-      <c r="E15" s="63">
+      <c r="E15" s="62">
         <v>44.2171995934142</v>
       </c>
-      <c r="F15" s="63">
+      <c r="F15" s="62">
         <v>0.43902393600891298</v>
       </c>
-      <c r="G15" s="63">
+      <c r="G15" s="62">
         <v>0.41270348255525702</v>
       </c>
-      <c r="H15" s="63">
+      <c r="H15" s="62">
         <f t="shared" si="0"/>
         <v>5.9952206007103936E-2</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="104">
+      <c r="A16" s="102">
         <v>41</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="53" t="s">
         <v>197</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="53" t="s">
         <v>196</v>
       </c>
-      <c r="D16" s="58">
+      <c r="D16" s="57">
         <v>82.851148258007399</v>
       </c>
-      <c r="E16" s="58">
+      <c r="E16" s="57">
         <v>57.944403738835199</v>
       </c>
-      <c r="F16" s="58">
+      <c r="F16" s="57">
         <v>0.45433700239720098</v>
       </c>
-      <c r="G16" s="58">
+      <c r="G16" s="57">
         <v>0.47323462504554298</v>
       </c>
-      <c r="H16" s="58">
+      <c r="H16" s="57">
         <f t="shared" si="0"/>
         <v>-4.1593844544100866E-2</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="106"/>
-      <c r="B17" s="106"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="72"/>
+      <c r="A17" s="104"/>
+      <c r="B17" s="104"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="105" t="s">
+      <c r="A18" s="103" t="s">
         <v>242</v>
       </c>
-      <c r="B18" s="105"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="59">
+      <c r="B18" s="103"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="58">
         <f>AVERAGE(D3:D16)</f>
         <v>47.440722663641665</v>
       </c>
-      <c r="E18" s="59">
+      <c r="E18" s="58">
         <f>AVERAGE(E3:E16)</f>
         <v>40.736750892549104</v>
       </c>
-      <c r="F18" s="59">
+      <c r="F18" s="58">
         <f>AVERAGE(F3:F16)</f>
         <v>0.46881605842755125</v>
       </c>
-      <c r="G18" s="59">
+      <c r="G18" s="58">
         <f>AVERAGE(G3:G16)</f>
         <v>0.4680067707906585</v>
       </c>
-      <c r="H18" s="59">
+      <c r="H18" s="58">
         <f>AVERAGE(H3:H16)</f>
         <v>-2.7663290336526987E-2</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="104" t="s">
+      <c r="A19" s="102" t="s">
         <v>241</v>
       </c>
-      <c r="B19" s="104"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="58">
+      <c r="B19" s="102"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="57">
         <f>STDEVA(D3:D16)</f>
         <v>27.133609361472772</v>
       </c>
-      <c r="E19" s="58">
+      <c r="E19" s="57">
         <f>STDEVA(E3:E16)</f>
         <v>20.980669470192939</v>
       </c>
-      <c r="F19" s="58">
+      <c r="F19" s="57">
         <f>STDEVA(F3:F16)</f>
         <v>0.11372731760468602</v>
       </c>
-      <c r="G19" s="58">
+      <c r="G19" s="57">
         <f>STDEVA(G3:G16)</f>
         <v>7.3753648264822308E-2</v>
       </c>
-      <c r="H19" s="58">
+      <c r="H19" s="57">
         <f>STDEVA(H3:H16)</f>
         <v>0.14926093687360459</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="105" t="s">
+      <c r="A20" s="103" t="s">
         <v>240</v>
       </c>
-      <c r="B20" s="105"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="59">
+      <c r="B20" s="103"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="58">
         <f>D19/SQRT(COUNT(D3:D16)-1)</f>
         <v>7.5255092185538306</v>
       </c>
-      <c r="E20" s="59">
+      <c r="E20" s="58">
         <f>E19/SQRT(COUNT(E3:E16)-1)</f>
         <v>5.8189907360263486</v>
       </c>
-      <c r="F20" s="59">
+      <c r="F20" s="58">
         <f>F19/SQRT(COUNT(F3:F16)-1)</f>
         <v>3.1542282695744148E-2</v>
       </c>
-      <c r="G20" s="59">
+      <c r="G20" s="58">
         <f>G19/SQRT(COUNT(G3:G16)-1)</f>
         <v>2.0455581582411734E-2</v>
       </c>
-      <c r="H20" s="59">
+      <c r="H20" s="58">
         <f>H19/SQRT(COUNT(H3:H16)-1)</f>
         <v>4.1397535486275006E-2</v>
       </c>
@@ -7998,8 +8013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE29F74-13EB-B64A-A652-3C18F5FB9619}">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:B42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8025,856 +8040,968 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:19" ht="19">
-      <c r="A2" s="51"/>
-      <c r="B2" s="54"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="53"/>
       <c r="C2" s="19"/>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="60" t="s">
         <v>290</v>
       </c>
-      <c r="E2" s="61" t="s">
+      <c r="E2" s="60" t="s">
         <v>290</v>
       </c>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="65" t="s">
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="64" t="s">
         <v>291</v>
       </c>
-      <c r="J2" s="58" t="s">
+      <c r="J2" s="57" t="s">
         <v>289</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="K2" s="57" t="s">
         <v>289</v>
       </c>
-      <c r="L2" s="61" t="s">
+      <c r="L2" s="60" t="s">
         <v>290</v>
       </c>
-      <c r="M2" s="45" t="s">
+      <c r="M2" s="44" t="s">
         <v>290</v>
       </c>
       <c r="N2" s="27"/>
       <c r="O2" s="27"/>
     </row>
-    <row r="3" spans="1:19" s="36" customFormat="1" ht="34">
-      <c r="A3" s="52" t="s">
+    <row r="3" spans="1:19" s="36" customFormat="1" ht="51">
+      <c r="A3" s="51" t="s">
         <v>239</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="51" t="s">
         <v>238</v>
       </c>
       <c r="C3" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="56" t="s">
         <v>236</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="56" t="s">
         <v>235</v>
       </c>
-      <c r="F3" s="62" t="s">
+      <c r="F3" s="61" t="s">
         <v>293</v>
       </c>
-      <c r="G3" s="62" t="s">
+      <c r="G3" s="61" t="s">
         <v>292</v>
       </c>
-      <c r="H3" s="57" t="s">
+      <c r="H3" s="56" t="s">
         <v>243</v>
       </c>
-      <c r="I3" s="57" t="s">
+      <c r="I3" s="56" t="s">
         <v>261</v>
       </c>
-      <c r="J3" s="57" t="s">
+      <c r="J3" s="56" t="s">
         <v>285</v>
       </c>
-      <c r="K3" s="57" t="s">
+      <c r="K3" s="56" t="s">
         <v>286</v>
       </c>
-      <c r="L3" s="57" t="s">
+      <c r="L3" s="56" t="s">
         <v>287</v>
       </c>
-      <c r="M3" s="46" t="s">
+      <c r="M3" s="45" t="s">
         <v>288</v>
       </c>
-      <c r="N3" s="37"/>
-      <c r="O3" s="33"/>
+      <c r="N3" s="37" t="s">
+        <v>313</v>
+      </c>
+      <c r="O3" s="33" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="75">
+      <c r="A4" s="74">
         <v>2</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="75" t="s">
         <v>231</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="75" t="s">
         <v>222</v>
       </c>
-      <c r="D4" s="77">
+      <c r="D4" s="76">
         <v>29.014212707890501</v>
       </c>
-      <c r="E4" s="77">
+      <c r="E4" s="76">
         <v>49.1064179566864</v>
       </c>
-      <c r="F4" s="77">
+      <c r="F4" s="76">
         <v>2.0626883146966799</v>
       </c>
-      <c r="G4" s="77">
+      <c r="G4" s="76">
         <v>0.54245987176745303</v>
       </c>
-      <c r="H4" s="77">
+      <c r="H4" s="76">
         <f t="shared" ref="H4:H13" si="0">1-G4/F4</f>
         <v>0.73701316485752133</v>
       </c>
-      <c r="I4" s="78">
-        <f>(D4-(1-H4)*E4)/H4</f>
+      <c r="I4" s="77">
+        <f t="shared" ref="I4:I15" si="1">(D4-(1-H4)*E4)/H4</f>
         <v>21.844753977210395</v>
       </c>
-      <c r="J4" s="77">
+      <c r="J4" s="76">
         <f>$B$42*(1/H4-1)*1000000</f>
         <v>19.143125881113672</v>
       </c>
-      <c r="K4" s="77">
+      <c r="K4" s="76">
         <f>$B$40*(1/H4-1)*1000000</f>
         <v>239.28907351392087</v>
       </c>
-      <c r="L4" s="77">
-        <f>E4/(1+3*0.000000000001*E4/(1000000000*0.000001*J4*$B$31*$B$24))</f>
+      <c r="L4" s="76">
+        <f t="shared" ref="L4:L15" si="2">E4/(1+3*0.000000000001*E4/(1000000000*0.000001*J4*$B$31*$B$24))</f>
         <v>0.31447284726731756</v>
       </c>
-      <c r="M4" s="77">
-        <f>E4/(1+3*0.000000000001*E4/(1000000000*0.000001*K4*$B$31*$B$24))</f>
+      <c r="M4" s="76">
+        <f t="shared" ref="M4:M15" si="3">E4/(1+3*0.000000000001*E4/(1000000000*0.000001*K4*$B$31*$B$24))</f>
         <v>3.6612762313493632</v>
+      </c>
+      <c r="N4" s="22">
+        <f>K4*0.000001*$B$27</f>
+        <v>239289.07351392086</v>
+      </c>
+      <c r="O4" s="1">
+        <f>I4/E4</f>
+        <v>0.44484519307594866</v>
       </c>
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="22"/>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="51">
+      <c r="A5" s="50">
         <v>5</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="53" t="s">
         <v>262</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="D5" s="58">
+      <c r="D5" s="57">
         <v>7.2400556486003396</v>
       </c>
-      <c r="E5" s="58">
+      <c r="E5" s="57">
         <v>41.862826268845801</v>
       </c>
-      <c r="F5" s="58">
+      <c r="F5" s="57">
         <v>1.8918624523762799</v>
       </c>
-      <c r="G5" s="58">
+      <c r="G5" s="57">
         <v>0.46080653045959202</v>
       </c>
-      <c r="H5" s="58">
+      <c r="H5" s="57">
         <f t="shared" si="0"/>
         <v>0.75642704368872349</v>
       </c>
-      <c r="I5" s="67">
-        <f>(D5-(1-H5)*E5)/H5</f>
+      <c r="I5" s="66">
+        <f t="shared" si="1"/>
         <v>-3.9086343222605131</v>
       </c>
-      <c r="J5" s="58">
-        <f t="shared" ref="J5:J15" si="1">$B$42*(1/H5-1)*1000000</f>
+      <c r="J5" s="57">
+        <f t="shared" ref="J5:J15" si="4">$B$42*(1/H5-1)*1000000</f>
         <v>17.274922671332416</v>
       </c>
-      <c r="K5" s="58">
-        <f t="shared" ref="K5:K14" si="2">$B$40*(1/H5-1)*1000000</f>
+      <c r="K5" s="57">
+        <f t="shared" ref="K5:K14" si="5">$B$40*(1/H5-1)*1000000</f>
         <v>215.93653339165516</v>
       </c>
-      <c r="L5" s="58">
-        <f>E5/(1+3*0.000000000001*E5/(1000000000*0.000001*J5*$B$31*$B$24))</f>
+      <c r="L5" s="57">
+        <f t="shared" si="2"/>
         <v>0.28367665107611295</v>
       </c>
-      <c r="M5" s="48">
-        <f>E5/(1+3*0.000000000001*E5/(1000000000*0.000001*K5*$B$31*$B$24))</f>
+      <c r="M5" s="47">
+        <f t="shared" si="3"/>
         <v>3.2896060948713481</v>
+      </c>
+      <c r="N5" s="22">
+        <f t="shared" ref="N5:N15" si="6">K5*0.000001*$B$27</f>
+        <v>215936.53339165516</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" ref="O5:O15" si="7">I5/E5</f>
+        <v>-9.3367664599590297E-2</v>
       </c>
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="22"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="53">
+      <c r="A6" s="52">
         <v>8</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="54" t="s">
         <v>230</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="D6" s="63">
+      <c r="D6" s="62">
         <v>13.931415193039999</v>
       </c>
-      <c r="E6" s="63">
+      <c r="E6" s="62">
         <v>22.884319607715199</v>
       </c>
-      <c r="F6" s="63">
+      <c r="F6" s="62">
         <v>1.3133947096291301</v>
       </c>
-      <c r="G6" s="63">
+      <c r="G6" s="62">
         <v>0.53835226307426698</v>
       </c>
-      <c r="H6" s="63">
+      <c r="H6" s="62">
         <f t="shared" si="0"/>
         <v>0.59010626498847074</v>
       </c>
-      <c r="I6" s="66">
-        <f>(D6-(1-H6)*E6)/H6</f>
+      <c r="I6" s="65">
+        <f t="shared" si="1"/>
         <v>7.7126379194177215</v>
       </c>
-      <c r="J6" s="63">
-        <f t="shared" si="1"/>
+      <c r="J6" s="62">
+        <f t="shared" si="4"/>
         <v>37.264487004789601</v>
       </c>
-      <c r="K6" s="63">
+      <c r="K6" s="62">
+        <f t="shared" si="5"/>
+        <v>465.80608755986998</v>
+      </c>
+      <c r="L6" s="62">
         <f t="shared" si="2"/>
-        <v>465.80608755986998</v>
-      </c>
-      <c r="L6" s="63">
-        <f>E6/(1+3*0.000000000001*E6/(1000000000*0.000001*J6*$B$31*$B$24))</f>
         <v>0.59995384668523477</v>
       </c>
-      <c r="M6" s="47">
-        <f>E6/(1+3*0.000000000001*E6/(1000000000*0.000001*K6*$B$31*$B$24))</f>
+      <c r="M6" s="46">
+        <f t="shared" si="3"/>
         <v>5.7621679905553931</v>
+      </c>
+      <c r="N6" s="22">
+        <f t="shared" si="6"/>
+        <v>465806.08755986998</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="7"/>
+        <v>0.33702718943050813</v>
       </c>
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="51">
+      <c r="A7" s="50">
         <v>11</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="53" t="s">
         <v>229</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="D7" s="58">
+      <c r="D7" s="57">
         <v>13.379041253793799</v>
       </c>
-      <c r="E7" s="58">
+      <c r="E7" s="57">
         <v>36.095885683268797</v>
       </c>
-      <c r="F7" s="58">
+      <c r="F7" s="57">
         <v>1.5275522267813499</v>
       </c>
-      <c r="G7" s="58">
+      <c r="G7" s="57">
         <v>0.42015490295138203</v>
       </c>
-      <c r="H7" s="58">
+      <c r="H7" s="57">
         <f t="shared" si="0"/>
         <v>0.72494891134643868</v>
       </c>
-      <c r="I7" s="67">
-        <f>(D7-(1-H7)*E7)/H7</f>
+      <c r="I7" s="66">
+        <f t="shared" si="1"/>
         <v>4.7600990175804778</v>
       </c>
-      <c r="J7" s="58">
-        <f t="shared" si="1"/>
+      <c r="J7" s="57">
+        <f t="shared" si="4"/>
         <v>20.354482172141761</v>
       </c>
-      <c r="K7" s="58">
+      <c r="K7" s="57">
+        <f t="shared" si="5"/>
+        <v>254.43102715177199</v>
+      </c>
+      <c r="L7" s="57">
         <f t="shared" si="2"/>
-        <v>254.43102715177199</v>
-      </c>
-      <c r="L7" s="58">
-        <f>E7/(1+3*0.000000000001*E7/(1000000000*0.000001*J7*$B$31*$B$24))</f>
         <v>0.33341892318851241</v>
       </c>
-      <c r="M7" s="48">
-        <f>E7/(1+3*0.000000000001*E7/(1000000000*0.000001*K7*$B$31*$B$24))</f>
+      <c r="M7" s="47">
+        <f t="shared" si="3"/>
         <v>3.7675275673058639</v>
+      </c>
+      <c r="N7" s="22">
+        <f t="shared" si="6"/>
+        <v>254431.027151772</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="7"/>
+        <v>0.13187372819575621</v>
       </c>
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="53">
+      <c r="A8" s="52">
         <v>14</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="54" t="s">
         <v>228</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="D8" s="63">
+      <c r="D8" s="62">
         <v>20.223851717782502</v>
       </c>
-      <c r="E8" s="63">
+      <c r="E8" s="62">
         <v>46.031094424366202</v>
       </c>
-      <c r="F8" s="63">
+      <c r="F8" s="62">
         <v>1.7673394447689299</v>
       </c>
-      <c r="G8" s="63">
+      <c r="G8" s="62">
         <v>0.40777654058540003</v>
       </c>
-      <c r="H8" s="63">
+      <c r="H8" s="62">
         <f t="shared" si="0"/>
         <v>0.7692709559601808</v>
       </c>
-      <c r="I8" s="66">
-        <f>(D8-(1-H8)*E8)/H8</f>
+      <c r="I8" s="65">
+        <f t="shared" si="1"/>
         <v>12.483431527913964</v>
       </c>
-      <c r="J8" s="63">
-        <f t="shared" si="1"/>
+      <c r="J8" s="62">
+        <f t="shared" si="4"/>
         <v>16.090777251888692</v>
       </c>
-      <c r="K8" s="63">
+      <c r="K8" s="62">
+        <f t="shared" si="5"/>
+        <v>201.13471564860865</v>
+      </c>
+      <c r="L8" s="62">
         <f t="shared" si="2"/>
-        <v>201.13471564860865</v>
-      </c>
-      <c r="L8" s="63">
-        <f>E8/(1+3*0.000000000001*E8/(1000000000*0.000001*J8*$B$31*$B$24))</f>
         <v>0.26450548894142906</v>
       </c>
-      <c r="M8" s="47">
-        <f>E8/(1+3*0.000000000001*E8/(1000000000*0.000001*K8*$B$31*$B$24))</f>
+      <c r="M8" s="46">
+        <f t="shared" si="3"/>
         <v>3.1013745021927597</v>
+      </c>
+      <c r="N8" s="22">
+        <f t="shared" si="6"/>
+        <v>201134.71564860863</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="7"/>
+        <v>0.27119562730418068</v>
       </c>
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="51">
+      <c r="A9" s="50">
         <v>16</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="53" t="s">
         <v>227</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="D9" s="58">
+      <c r="D9" s="57">
         <v>12.4570649430594</v>
       </c>
-      <c r="E9" s="58">
+      <c r="E9" s="57">
         <v>22.326414077468499</v>
       </c>
-      <c r="F9" s="58">
+      <c r="F9" s="57">
         <v>1.7748817210721599</v>
       </c>
-      <c r="G9" s="58">
+      <c r="G9" s="57">
         <v>0.55606217067729802</v>
       </c>
-      <c r="H9" s="58">
+      <c r="H9" s="57">
         <f t="shared" si="0"/>
         <v>0.68670466089346205</v>
       </c>
-      <c r="I9" s="67">
-        <f>(D9-(1-H9)*E9)/H9</f>
+      <c r="I9" s="66">
+        <f t="shared" si="1"/>
         <v>7.9543707574650746</v>
       </c>
-      <c r="J9" s="58">
-        <f t="shared" si="1"/>
+      <c r="J9" s="57">
+        <f t="shared" si="4"/>
         <v>24.475863968015485</v>
       </c>
-      <c r="K9" s="58">
+      <c r="K9" s="57">
+        <f t="shared" si="5"/>
+        <v>305.94829960019354</v>
+      </c>
+      <c r="L9" s="57">
         <f t="shared" si="2"/>
-        <v>305.94829960019354</v>
-      </c>
-      <c r="L9" s="58">
-        <f>E9/(1+3*0.000000000001*E9/(1000000000*0.000001*J9*$B$31*$B$24))</f>
         <v>0.39746356621205353</v>
       </c>
-      <c r="M9" s="48">
-        <f>E9/(1+3*0.000000000001*E9/(1000000000*0.000001*K9*$B$31*$B$24))</f>
+      <c r="M9" s="47">
+        <f t="shared" si="3"/>
         <v>4.1239986337938133</v>
+      </c>
+      <c r="N9" s="22">
+        <f t="shared" si="6"/>
+        <v>305948.29960019351</v>
+      </c>
+      <c r="O9" s="1">
+        <f t="shared" si="7"/>
+        <v>0.3562762353983443</v>
       </c>
       <c r="Q9" s="22"/>
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="53">
+      <c r="A10" s="52">
         <v>19</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="54" t="s">
         <v>226</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="D10" s="63">
+      <c r="D10" s="62">
         <v>10.946419715329601</v>
       </c>
-      <c r="E10" s="63">
+      <c r="E10" s="62">
         <v>41.3677583378227</v>
       </c>
-      <c r="F10" s="63">
+      <c r="F10" s="62">
         <v>1.63158333583306</v>
       </c>
-      <c r="G10" s="63">
+      <c r="G10" s="62">
         <v>0.474038139416954</v>
       </c>
-      <c r="H10" s="63">
+      <c r="H10" s="62">
         <f t="shared" si="0"/>
         <v>0.70946127665926562</v>
       </c>
-      <c r="I10" s="66">
-        <f>(D10-(1-H10)*E10)/H10</f>
+      <c r="I10" s="65">
+        <f t="shared" si="1"/>
         <v>-1.5117329372220647</v>
       </c>
-      <c r="J10" s="63">
-        <f t="shared" si="1"/>
+      <c r="J10" s="62">
+        <f t="shared" si="4"/>
         <v>21.96996776813037</v>
       </c>
-      <c r="K10" s="63">
+      <c r="K10" s="62">
+        <f t="shared" si="5"/>
+        <v>274.6245971016296</v>
+      </c>
+      <c r="L10" s="62">
         <f t="shared" si="2"/>
-        <v>274.6245971016296</v>
-      </c>
-      <c r="L10" s="63">
-        <f>E10/(1+3*0.000000000001*E10/(1000000000*0.000001*J10*$B$31*$B$24))</f>
         <v>0.36007509837561946</v>
       </c>
-      <c r="M10" s="47">
-        <f>E10/(1+3*0.000000000001*E10/(1000000000*0.000001*K10*$B$31*$B$24))</f>
+      <c r="M10" s="46">
+        <f t="shared" si="3"/>
         <v>4.0913949402737453</v>
+      </c>
+      <c r="N10" s="22">
+        <f t="shared" si="6"/>
+        <v>274624.5971016296</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="7"/>
+        <v>-3.6543748029002614E-2</v>
       </c>
       <c r="Q10" s="22"/>
       <c r="R10" s="22"/>
       <c r="S10" s="22"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="51">
+      <c r="A11" s="50">
         <v>21</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="53" t="s">
         <v>225</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="D11" s="58">
+      <c r="D11" s="57">
         <v>42.3764290443196</v>
       </c>
-      <c r="E11" s="58">
+      <c r="E11" s="57">
         <v>70.394190376426295</v>
       </c>
-      <c r="F11" s="58">
+      <c r="F11" s="57">
         <v>1.0268209712124701</v>
       </c>
-      <c r="G11" s="58">
+      <c r="G11" s="57">
         <v>0.63364791058390801</v>
       </c>
-      <c r="H11" s="58">
+      <c r="H11" s="57">
         <f t="shared" si="0"/>
         <v>0.38290322427316936</v>
       </c>
-      <c r="I11" s="67">
-        <f>(D11-(1-H11)*E11)/H11</f>
+      <c r="I11" s="66">
+        <f t="shared" si="1"/>
         <v>-2.7777224098665863</v>
       </c>
-      <c r="J11" s="58">
-        <f t="shared" si="1"/>
+      <c r="J11" s="57">
+        <f t="shared" si="4"/>
         <v>86.460620076468388</v>
       </c>
-      <c r="K11" s="58">
+      <c r="K11" s="57">
+        <f t="shared" si="5"/>
+        <v>1080.7577509558548</v>
+      </c>
+      <c r="L11" s="57">
         <f t="shared" si="2"/>
-        <v>1080.7577509558548</v>
-      </c>
-      <c r="L11" s="58">
-        <f>E11/(1+3*0.000000000001*E11/(1000000000*0.000001*J11*$B$31*$B$24))</f>
         <v>1.4010317503928373</v>
       </c>
-      <c r="M11" s="48">
-        <f>E11/(1+3*0.000000000001*E11/(1000000000*0.000001*K11*$B$31*$B$24))</f>
+      <c r="M11" s="47">
+        <f t="shared" si="3"/>
         <v>14.25109710293555</v>
+      </c>
+      <c r="N11" s="22">
+        <f t="shared" si="6"/>
+        <v>1080757.7509558548</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="7"/>
+        <v>-3.9459540553176013E-2</v>
       </c>
       <c r="Q11" s="22"/>
       <c r="R11" s="22"/>
       <c r="S11" s="22"/>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="53">
+      <c r="A12" s="52">
         <v>27</v>
       </c>
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="54" t="s">
         <v>263</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="D12" s="63">
+      <c r="D12" s="62">
         <v>10.042838094060301</v>
       </c>
-      <c r="E12" s="63">
+      <c r="E12" s="62">
         <v>19.441559166950402</v>
       </c>
-      <c r="F12" s="63">
+      <c r="F12" s="62">
         <v>1.65164503094854</v>
       </c>
-      <c r="G12" s="63">
+      <c r="G12" s="62">
         <v>0.36160354985295601</v>
       </c>
-      <c r="H12" s="63">
+      <c r="H12" s="62">
         <f t="shared" si="0"/>
         <v>0.78106460947889811</v>
       </c>
-      <c r="I12" s="66">
-        <f>(D12-(1-H12)*E12)/H12</f>
+      <c r="I12" s="65">
+        <f t="shared" si="1"/>
         <v>7.4083407125121266</v>
       </c>
-      <c r="J12" s="63">
-        <f t="shared" si="1"/>
+      <c r="J12" s="62">
+        <f t="shared" si="4"/>
         <v>15.037758365088628</v>
       </c>
-      <c r="K12" s="63">
+      <c r="K12" s="62">
+        <f t="shared" si="5"/>
+        <v>187.97197956360782</v>
+      </c>
+      <c r="L12" s="62">
         <f t="shared" si="2"/>
-        <v>187.97197956360782</v>
-      </c>
-      <c r="L12" s="63">
-        <f>E12/(1+3*0.000000000001*E12/(1000000000*0.000001*J12*$B$31*$B$24))</f>
         <v>0.24548493935721266</v>
       </c>
-      <c r="M12" s="47">
-        <f>E12/(1+3*0.000000000001*E12/(1000000000*0.000001*K12*$B$31*$B$24))</f>
+      <c r="M12" s="46">
+        <f t="shared" si="3"/>
         <v>2.6794790063230218</v>
+      </c>
+      <c r="N12" s="22">
+        <f t="shared" si="6"/>
+        <v>187971.97956360783</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="7"/>
+        <v>0.38105692289875109</v>
       </c>
       <c r="Q12" s="22"/>
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
     </row>
     <row r="13" spans="1:19" s="24" customFormat="1">
-      <c r="A13" s="51">
+      <c r="A13" s="50">
         <v>32</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="53" t="s">
         <v>264</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="D13" s="58">
+      <c r="D13" s="57">
         <v>4.81046503051736</v>
       </c>
-      <c r="E13" s="58">
+      <c r="E13" s="57">
         <v>35.869121816015401</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="57">
         <v>2.1967906677561801</v>
       </c>
-      <c r="G13" s="58">
+      <c r="G13" s="57">
         <v>0.38637956223555497</v>
       </c>
-      <c r="H13" s="64">
+      <c r="H13" s="63">
         <f t="shared" si="0"/>
         <v>0.82411634940610601</v>
       </c>
-      <c r="I13" s="68">
-        <f>(D13-(1-H13)*E13)/H13</f>
+      <c r="I13" s="67">
+        <f t="shared" si="1"/>
         <v>-1.8181013629450173</v>
       </c>
-      <c r="J13" s="58">
-        <f t="shared" si="1"/>
+      <c r="J13" s="57">
+        <f t="shared" si="4"/>
         <v>11.449618942408234</v>
       </c>
-      <c r="K13" s="58">
+      <c r="K13" s="57">
+        <f t="shared" si="5"/>
+        <v>143.12023678010294</v>
+      </c>
+      <c r="L13" s="57">
         <f t="shared" si="2"/>
-        <v>143.12023678010294</v>
-      </c>
-      <c r="L13" s="58">
-        <f>E13/(1+3*0.000000000001*E13/(1000000000*0.000001*J13*$B$31*$B$24))</f>
         <v>0.18830657292636849</v>
       </c>
-      <c r="M13" s="48">
-        <f>E13/(1+3*0.000000000001*E13/(1000000000*0.000001*K13*$B$31*$B$24))</f>
+      <c r="M13" s="47">
+        <f t="shared" si="3"/>
         <v>2.2198153078655918</v>
       </c>
-      <c r="N13" s="22"/>
-      <c r="O13" s="1"/>
+      <c r="N13" s="22">
+        <f t="shared" si="6"/>
+        <v>143120.23678010292</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="7"/>
+        <v>-5.0687088807767892E-2</v>
+      </c>
       <c r="P13" s="25"/>
       <c r="Q13" s="22"/>
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
     </row>
     <row r="14" spans="1:19" s="24" customFormat="1">
-      <c r="A14" s="53">
+      <c r="A14" s="52">
         <v>34</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="54" t="s">
         <v>224</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="D14" s="63">
+      <c r="D14" s="62">
         <v>7.3615758218360599</v>
       </c>
-      <c r="E14" s="63">
+      <c r="E14" s="62">
         <v>20.183808492096901</v>
       </c>
-      <c r="F14" s="63">
+      <c r="F14" s="62">
         <v>1.83909319932013</v>
       </c>
-      <c r="G14" s="63">
+      <c r="G14" s="62">
         <v>0.35668134024120202</v>
       </c>
-      <c r="H14" s="63">
-        <f t="shared" ref="H14:H15" si="3">1-G14/F14</f>
+      <c r="H14" s="62">
+        <f t="shared" ref="H14:H15" si="8">1-G14/F14</f>
         <v>0.80605586472014645</v>
       </c>
-      <c r="I14" s="66">
-        <f>(D14-(1-H14)*E14)/H14</f>
+      <c r="I14" s="65">
+        <f t="shared" si="1"/>
         <v>4.276433790825326</v>
       </c>
-      <c r="J14" s="63">
-        <f t="shared" si="1"/>
+      <c r="J14" s="62">
+        <f t="shared" si="4"/>
         <v>12.908197487227758</v>
       </c>
-      <c r="K14" s="63">
+      <c r="K14" s="62">
+        <f t="shared" si="5"/>
+        <v>161.35246859034697</v>
+      </c>
+      <c r="L14" s="62">
         <f t="shared" si="2"/>
-        <v>161.35246859034697</v>
-      </c>
-      <c r="L14" s="63">
-        <f>E14/(1+3*0.000000000001*E14/(1000000000*0.000001*J14*$B$31*$B$24))</f>
         <v>0.21118257159996667</v>
       </c>
-      <c r="M14" s="47">
-        <f>E14/(1+3*0.000000000001*E14/(1000000000*0.000001*K14*$B$31*$B$24))</f>
+      <c r="M14" s="46">
+        <f t="shared" si="3"/>
         <v>2.356266396803079</v>
       </c>
-      <c r="N14" s="22"/>
-      <c r="O14" s="1"/>
+      <c r="N14" s="22">
+        <f t="shared" si="6"/>
+        <v>161352.46859034698</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="7"/>
+        <v>0.21187447316990701</v>
+      </c>
       <c r="P14" s="25"/>
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="22"/>
     </row>
     <row r="15" spans="1:19" s="24" customFormat="1">
-      <c r="A15" s="51">
+      <c r="A15" s="50">
         <v>39</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="53" t="s">
         <v>223</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="D15" s="58">
+      <c r="D15" s="57">
         <v>10.9503916311275</v>
       </c>
-      <c r="E15" s="58">
+      <c r="E15" s="57">
         <v>10.9011360963647</v>
       </c>
-      <c r="F15" s="58">
+      <c r="F15" s="57">
         <v>2.94937457599179</v>
       </c>
-      <c r="G15" s="58">
+      <c r="G15" s="57">
         <v>0.457887359531786</v>
       </c>
-      <c r="H15" s="58">
-        <f t="shared" si="3"/>
+      <c r="H15" s="57">
+        <f t="shared" si="8"/>
         <v>0.84475103187671186</v>
       </c>
-      <c r="I15" s="67">
-        <f>(D15-(1-H15)*E15)/H15</f>
+      <c r="I15" s="66">
+        <f t="shared" si="1"/>
         <v>10.959443849660218</v>
       </c>
-      <c r="J15" s="58">
-        <f t="shared" si="1"/>
+      <c r="J15" s="57">
+        <f t="shared" si="4"/>
         <v>9.8594816560899634</v>
       </c>
-      <c r="K15" s="58">
+      <c r="K15" s="57">
         <f>$B$40*(1/H15-1)*1000000</f>
         <v>123.24352070112454</v>
       </c>
-      <c r="L15" s="58">
-        <f>E15/(1+3*0.000000000001*E15/(1000000000*0.000001*J15*$B$31*$B$24))</f>
+      <c r="L15" s="57">
+        <f t="shared" si="2"/>
         <v>0.16060843903822675</v>
       </c>
-      <c r="M15" s="48">
-        <f>E15/(1+3*0.000000000001*E15/(1000000000*0.000001*K15*$B$31*$B$24))</f>
+      <c r="M15" s="47">
+        <f t="shared" si="3"/>
         <v>1.7167361215015471</v>
       </c>
-      <c r="N15" s="22"/>
-      <c r="O15" s="1"/>
+      <c r="N15" s="22">
+        <f t="shared" si="6"/>
+        <v>123243.52070112454</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="7"/>
+        <v>1.005348777666849</v>
+      </c>
       <c r="P15" s="25"/>
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
     </row>
     <row r="16" spans="1:19" s="19" customFormat="1">
-      <c r="A16" s="69"/>
-      <c r="B16" s="70"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="74"/>
+      <c r="A16" s="68"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="71"/>
+      <c r="M16" s="73"/>
       <c r="N16" s="23"/>
       <c r="O16" s="2"/>
     </row>
     <row r="17" spans="1:19" s="39" customFormat="1" ht="17">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="B17" s="56"/>
-      <c r="D17" s="59">
+      <c r="B17" s="55"/>
+      <c r="D17" s="58">
         <f>AVERAGE(D4:D15)</f>
         <v>15.227813400113078</v>
       </c>
-      <c r="E17" s="59">
+      <c r="E17" s="58">
         <f>AVERAGE(E4:E15)</f>
         <v>34.70537769200228</v>
       </c>
-      <c r="F17" s="59">
-        <f t="shared" ref="F17:K17" si="4">AVERAGE(F4:F15)</f>
+      <c r="F17" s="58">
+        <f t="shared" ref="F17:K17" si="9">AVERAGE(F4:F15)</f>
         <v>1.802752220865558</v>
       </c>
-      <c r="G17" s="59">
-        <f t="shared" si="4"/>
+      <c r="G17" s="58">
+        <f t="shared" si="9"/>
         <v>0.4663208451148127</v>
       </c>
-      <c r="H17" s="59">
-        <f t="shared" si="4"/>
+      <c r="H17" s="58">
+        <f t="shared" si="9"/>
         <v>0.71773527984575791</v>
       </c>
-      <c r="I17" s="59">
-        <f t="shared" si="4"/>
+      <c r="I17" s="58">
+        <f t="shared" si="9"/>
         <v>5.6152767100242604</v>
       </c>
-      <c r="J17" s="59">
-        <f t="shared" si="4"/>
+      <c r="J17" s="58">
+        <f t="shared" si="9"/>
         <v>24.357441937057914</v>
       </c>
-      <c r="K17" s="59">
-        <f t="shared" si="4"/>
+      <c r="K17" s="58">
+        <f t="shared" si="9"/>
         <v>304.46802421322394</v>
       </c>
-      <c r="L17" s="59">
-        <f t="shared" ref="L17:M17" si="5">AVERAGE(L4:L15)</f>
+      <c r="L17" s="58">
+        <f t="shared" ref="L17:M17" si="10">AVERAGE(L4:L15)</f>
         <v>0.39668172458840761</v>
       </c>
-      <c r="M17" s="49">
-        <f t="shared" si="5"/>
+      <c r="M17" s="48">
+        <f t="shared" si="10"/>
         <v>4.2517283246475897</v>
       </c>
-      <c r="N17" s="40"/>
-      <c r="O17" s="26"/>
+      <c r="N17" s="118">
+        <f t="shared" ref="N17:O17" si="11">AVERAGE(N4:N15)</f>
+        <v>304468.02421322389</v>
+      </c>
+      <c r="O17" s="122">
+        <f t="shared" si="11"/>
+        <v>0.24328667542922569</v>
+      </c>
       <c r="P17" s="26"/>
       <c r="Q17" s="26"/>
       <c r="R17" s="26"/>
       <c r="S17" s="26"/>
     </row>
     <row r="18" spans="1:19" s="19" customFormat="1" ht="17">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="50" t="s">
         <v>241</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="D18" s="58">
+      <c r="B18" s="53"/>
+      <c r="D18" s="57">
         <f>STDEVA(D4:D15)</f>
         <v>10.71346621738301</v>
       </c>
-      <c r="E18" s="58">
+      <c r="E18" s="57">
         <f>STDEVA(E4:E15)</f>
         <v>16.546726043182563</v>
       </c>
-      <c r="F18" s="58">
-        <f t="shared" ref="F18:K18" si="6">STDEVA(F4:F15)</f>
+      <c r="F18" s="57">
+        <f t="shared" ref="F18:K18" si="12">STDEVA(F4:F15)</f>
         <v>0.47847060421793908</v>
       </c>
-      <c r="G18" s="58">
-        <f t="shared" si="6"/>
+      <c r="G18" s="57">
+        <f t="shared" si="12"/>
         <v>8.6410483557239182E-2</v>
       </c>
-      <c r="H18" s="58">
-        <f t="shared" si="6"/>
+      <c r="H18" s="57">
+        <f t="shared" si="12"/>
         <v>0.1255065170617311</v>
       </c>
-      <c r="I18" s="67">
-        <f t="shared" si="6"/>
+      <c r="I18" s="66">
+        <f t="shared" si="12"/>
         <v>7.5192691244222463</v>
       </c>
-      <c r="J18" s="67">
-        <f t="shared" si="6"/>
+      <c r="J18" s="66">
+        <f t="shared" si="12"/>
         <v>20.857890711324373</v>
       </c>
-      <c r="K18" s="67">
-        <f t="shared" si="6"/>
+      <c r="K18" s="66">
+        <f t="shared" si="12"/>
         <v>260.72363389155453</v>
       </c>
-      <c r="L18" s="67">
-        <f t="shared" ref="L18:M18" si="7">STDEVA(L4:L15)</f>
+      <c r="L18" s="66">
+        <f t="shared" ref="L18:M18" si="13">STDEVA(L4:L15)</f>
         <v>0.33693829693811178</v>
       </c>
-      <c r="M18" s="50">
-        <f t="shared" si="7"/>
+      <c r="M18" s="49">
+        <f t="shared" si="13"/>
         <v>3.3270585231762109</v>
       </c>
-      <c r="N18" s="23"/>
-      <c r="O18" s="2"/>
+      <c r="N18" s="119">
+        <f t="shared" ref="N18:O18" si="14">STDEVA(N4:N15)</f>
+        <v>260723.63389155461</v>
+      </c>
+      <c r="O18" s="123">
+        <f t="shared" si="14"/>
+        <v>0.30660675695864809</v>
+      </c>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
     </row>
     <row r="19" spans="1:19" s="39" customFormat="1" ht="17">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="51" t="s">
         <v>240</v>
       </c>
-      <c r="B19" s="56"/>
-      <c r="D19" s="59">
+      <c r="B19" s="55"/>
+      <c r="D19" s="58">
         <f>D18/SQRT(COUNT(D4:D15)-1)</f>
         <v>3.2302316042915984</v>
       </c>
-      <c r="E19" s="59">
+      <c r="E19" s="58">
         <f>E18/SQRT(COUNT(E4:E15)-1)</f>
         <v>4.9890256176398733</v>
       </c>
-      <c r="F19" s="59">
-        <f t="shared" ref="F19:M19" si="8">F18/SQRT(COUNT(F4:F15)-1)</f>
+      <c r="F19" s="58">
+        <f t="shared" ref="F19:M19" si="15">F18/SQRT(COUNT(F4:F15)-1)</f>
         <v>0.1442643152186858</v>
       </c>
-      <c r="G19" s="59">
-        <f t="shared" si="8"/>
+      <c r="G19" s="58">
+        <f t="shared" si="15"/>
         <v>2.605374108295792E-2</v>
       </c>
-      <c r="H19" s="59">
-        <f t="shared" si="8"/>
+      <c r="H19" s="58">
+        <f t="shared" si="15"/>
         <v>3.7841638712554575E-2</v>
       </c>
-      <c r="I19" s="59">
-        <f t="shared" si="8"/>
+      <c r="I19" s="58">
+        <f t="shared" si="15"/>
         <v>2.2671449439466147</v>
       </c>
-      <c r="J19" s="59">
-        <f t="shared" si="8"/>
+      <c r="J19" s="58">
+        <f t="shared" si="15"/>
         <v>6.2888906734274581</v>
       </c>
-      <c r="K19" s="59">
-        <f t="shared" si="8"/>
+      <c r="K19" s="58">
+        <f t="shared" si="15"/>
         <v>78.611133417843192</v>
       </c>
-      <c r="L19" s="59">
-        <f t="shared" si="8"/>
+      <c r="L19" s="58">
+        <f t="shared" si="15"/>
         <v>0.10159071894955186</v>
       </c>
-      <c r="M19" s="49">
-        <f t="shared" si="8"/>
+      <c r="M19" s="48">
+        <f t="shared" si="15"/>
         <v>1.0031458888117679</v>
       </c>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
+      <c r="N19" s="118">
+        <f t="shared" ref="N19:O19" si="16">N18/SQRT(COUNT(N4:N15)-1)</f>
+        <v>78611.133417843215</v>
+      </c>
+      <c r="O19" s="122">
+        <f t="shared" si="16"/>
+        <v>9.244541554722957E-2</v>
+      </c>
       <c r="P19" s="28"/>
       <c r="Q19" s="28"/>
       <c r="R19" s="28"/>
@@ -9106,8 +9233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A544C46-8A4E-704E-9B4C-D59AC133C1EF}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9127,611 +9254,679 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="19">
-      <c r="A1" s="54"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="83" t="s">
+      <c r="A1" s="53"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="81" t="s">
         <v>290</v>
       </c>
-      <c r="E1" s="83" t="s">
+      <c r="E1" s="81" t="s">
         <v>290</v>
       </c>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="84" t="s">
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="82" t="s">
         <v>291</v>
       </c>
-      <c r="J1" s="85" t="s">
+      <c r="J1" s="83" t="s">
         <v>289</v>
       </c>
-      <c r="K1" s="85" t="s">
+      <c r="K1" s="83" t="s">
         <v>289</v>
       </c>
-      <c r="L1" s="83" t="s">
+      <c r="L1" s="81" t="s">
         <v>290</v>
       </c>
-      <c r="M1" s="83" t="s">
+      <c r="M1" s="81" t="s">
         <v>290</v>
       </c>
-      <c r="N1" s="87"/>
+      <c r="N1" s="85" t="s">
+        <v>312</v>
+      </c>
       <c r="O1" s="31"/>
     </row>
     <row r="2" spans="1:18" ht="34">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="92" t="s">
         <v>239</v>
       </c>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="93" t="s">
         <v>238</v>
       </c>
-      <c r="C2" s="94" t="s">
+      <c r="C2" s="92" t="s">
         <v>237</v>
       </c>
-      <c r="D2" s="96" t="s">
+      <c r="D2" s="94" t="s">
         <v>236</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="59" t="s">
         <v>235</v>
       </c>
-      <c r="F2" s="97" t="s">
+      <c r="F2" s="95" t="s">
         <v>293</v>
       </c>
-      <c r="G2" s="98" t="s">
+      <c r="G2" s="96" t="s">
         <v>292</v>
       </c>
-      <c r="H2" s="96" t="s">
+      <c r="H2" s="94" t="s">
         <v>243</v>
       </c>
-      <c r="I2" s="60" t="s">
+      <c r="I2" s="59" t="s">
         <v>261</v>
       </c>
-      <c r="J2" s="99" t="s">
+      <c r="J2" s="97" t="s">
         <v>285</v>
       </c>
-      <c r="K2" s="100" t="s">
+      <c r="K2" s="98" t="s">
         <v>286</v>
       </c>
-      <c r="L2" s="100" t="s">
+      <c r="L2" s="98" t="s">
         <v>287</v>
       </c>
-      <c r="M2" s="101" t="s">
+      <c r="M2" s="99" t="s">
         <v>288</v>
       </c>
-      <c r="N2" s="81"/>
+      <c r="N2" s="79" t="s">
+        <v>311</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="55">
+      <c r="A3" s="54">
         <v>6</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="D3" s="43">
+      <c r="D3" s="42">
         <v>12.781840829533801</v>
       </c>
-      <c r="E3" s="63">
+      <c r="E3" s="62">
         <v>44.560245626773103</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="42">
         <v>3.2258263894167198</v>
       </c>
-      <c r="G3" s="63">
+      <c r="G3" s="62">
         <v>0.69575783120323098</v>
       </c>
-      <c r="H3" s="43">
+      <c r="H3" s="42">
         <f t="shared" ref="H3:H9" si="0">1-G3/F3</f>
         <v>0.78431640540672898</v>
       </c>
-      <c r="I3" s="66">
-        <f>(D3-(1-H3)*E3)/H3</f>
+      <c r="I3" s="65">
+        <f t="shared" ref="I3:I9" si="1">(D3-(1-H3)*E3)/H3</f>
         <v>4.0429179536897761</v>
       </c>
-      <c r="J3" s="44">
+      <c r="J3" s="43">
         <f>$B$36*(1/H3-1)*1000000</f>
         <v>18.441231456248126</v>
       </c>
-      <c r="K3" s="102">
+      <c r="K3" s="100">
         <f>$B$34*(1/H3-1)*1000000</f>
         <v>184.41231456248124</v>
       </c>
-      <c r="L3" s="102">
+      <c r="L3" s="100">
         <f>E3/(1+3*0.000000000001*E3/(1000000000*0.000001*J3*$B$26*$B$18))</f>
         <v>0.6015579610445414</v>
       </c>
-      <c r="M3" s="103">
-        <f>E3/(1+3*0.000000000001*E3/($B$21*0.000001*K3*$B$26*$B$18))</f>
+      <c r="M3" s="101">
+        <f t="shared" ref="M3:M9" si="2">E3/(1+3*0.000000000001*E3/($B$21*0.000001*K3*$B$26*$B$18))</f>
         <v>5.3638746426734603</v>
       </c>
-      <c r="N3" s="79"/>
-      <c r="O3" s="2"/>
+      <c r="N3" s="115">
+        <f>K3*0.000001*$B$21</f>
+        <v>184412.31456248125</v>
+      </c>
+      <c r="O3" s="2">
+        <f>I3/E3</f>
+        <v>9.0729256466680522E-2</v>
+      </c>
       <c r="P3" s="22"/>
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="54">
+      <c r="A4" s="53">
         <v>9</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="53" t="s">
         <v>212</v>
       </c>
       <c r="D4" s="2">
         <v>10.307004300054</v>
       </c>
-      <c r="E4" s="58">
+      <c r="E4" s="57">
         <v>43.183541617449301</v>
       </c>
       <c r="F4" s="2">
         <v>2.8236604859550498</v>
       </c>
-      <c r="G4" s="58">
+      <c r="G4" s="57">
         <v>0.66212585946069202</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="0"/>
         <v>0.7655079770552724</v>
       </c>
-      <c r="I4" s="67">
-        <f>(D4-(1-H4)*E4)/H4</f>
+      <c r="I4" s="66">
+        <f t="shared" si="1"/>
         <v>0.2361938394894407</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J4:J9" si="1">$B$36*(1/H4-1)*1000000</f>
+        <f t="shared" ref="J4:J9" si="3">$B$36*(1/H4-1)*1000000</f>
         <v>20.541987357512102</v>
       </c>
-      <c r="K4" s="81">
-        <f t="shared" ref="K4:K9" si="2">$B$34*(1/H4-1)*1000000</f>
+      <c r="K4" s="79">
+        <f t="shared" ref="K4:K9" si="4">$B$34*(1/H4-1)*1000000</f>
         <v>205.41987357512102</v>
       </c>
-      <c r="L4" s="81">
+      <c r="L4" s="79">
         <f>E4/(1+3*0.000000000001*E4/(1000000000*0.000001*J4*$B$26*$B$18))</f>
         <v>0.66873617029779375</v>
       </c>
-      <c r="M4" s="81">
-        <f>E4/(1+3*0.000000000001*E4/($B$21*0.000001*K4*$B$26*$B$18))</f>
+      <c r="M4" s="79">
+        <f t="shared" si="2"/>
         <v>5.8693342008762439</v>
       </c>
-      <c r="N4" s="79"/>
-      <c r="O4" s="2"/>
+      <c r="N4" s="115">
+        <f t="shared" ref="N4:N9" si="5">K4*0.000001*$B$21</f>
+        <v>205419.87357512102</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" ref="O4:O9" si="6">I4/E4</f>
+        <v>5.469533777053644E-3</v>
+      </c>
       <c r="P4" s="22"/>
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="55">
+      <c r="A5" s="54">
         <v>12</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="41" t="s">
         <v>219</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="42">
         <v>8.3531381851342701</v>
       </c>
-      <c r="E5" s="63">
+      <c r="E5" s="62">
         <v>30.9104011446341</v>
       </c>
-      <c r="F5" s="43">
+      <c r="F5" s="42">
         <v>3.2373240457758201</v>
       </c>
-      <c r="G5" s="63">
+      <c r="G5" s="62">
         <v>0.50155578216534302</v>
       </c>
-      <c r="H5" s="43">
+      <c r="H5" s="42">
         <f t="shared" si="0"/>
         <v>0.84507087487278532</v>
       </c>
-      <c r="I5" s="66">
-        <f>(D5-(1-H5)*E5)/H5</f>
+      <c r="I5" s="65">
+        <f t="shared" si="1"/>
         <v>4.2176542636159375</v>
       </c>
-      <c r="J5" s="44">
-        <f t="shared" si="1"/>
+      <c r="J5" s="43">
+        <f t="shared" si="3"/>
         <v>12.29430659438167</v>
       </c>
-      <c r="K5" s="102">
+      <c r="K5" s="100">
+        <f t="shared" si="4"/>
+        <v>122.94306594381668</v>
+      </c>
+      <c r="L5" s="100">
+        <f t="shared" ref="L5:L9" si="7">E5/(1+3*0.000000000001*E5/(1000000000*0.000001*J5*$B$26*$B$18))</f>
+        <v>0.40125446346719529</v>
+      </c>
+      <c r="M5" s="100">
         <f t="shared" si="2"/>
-        <v>122.94306594381668</v>
-      </c>
-      <c r="L5" s="102">
-        <f t="shared" ref="L5:L9" si="3">E5/(1+3*0.000000000001*E5/(1000000000*0.000001*J5*$B$26*$B$18))</f>
-        <v>0.40125446346719529</v>
-      </c>
-      <c r="M5" s="102">
-        <f>E5/(1+3*0.000000000001*E5/($B$21*0.000001*K5*$B$26*$B$18))</f>
         <v>3.5927951250625303</v>
       </c>
-      <c r="N5" s="79"/>
-      <c r="O5" s="2"/>
+      <c r="N5" s="115">
+        <f t="shared" si="5"/>
+        <v>122943.06594381668</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="6"/>
+        <v>0.13644773627753784</v>
+      </c>
       <c r="P5" s="22"/>
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="54">
+      <c r="A6" s="53">
         <v>17</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="53" t="s">
         <v>212</v>
       </c>
       <c r="D6" s="2">
         <v>9.3986794868277492</v>
       </c>
-      <c r="E6" s="58">
+      <c r="E6" s="57">
         <v>42.569398411928901</v>
       </c>
       <c r="F6" s="2">
         <v>4.4140960179519704</v>
       </c>
-      <c r="G6" s="58">
+      <c r="G6" s="57">
         <v>0.66785551747885796</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" si="0"/>
         <v>0.84869936794244771</v>
       </c>
-      <c r="I6" s="67">
-        <f>(D6-(1-H6)*E6)/H6</f>
+      <c r="I6" s="66">
+        <f t="shared" si="1"/>
         <v>3.4852183382251867</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.955038210475269</v>
       </c>
-      <c r="K6" s="81">
+      <c r="K6" s="79">
+        <f t="shared" si="4"/>
+        <v>119.55038210475269</v>
+      </c>
+      <c r="L6" s="79">
+        <f t="shared" si="7"/>
+        <v>0.39167603260752387</v>
+      </c>
+      <c r="M6" s="79">
         <f t="shared" si="2"/>
-        <v>119.55038210475269</v>
-      </c>
-      <c r="L6" s="81">
-        <f t="shared" si="3"/>
-        <v>0.39167603260752387</v>
-      </c>
-      <c r="M6" s="81">
-        <f>E6/(1+3*0.000000000001*E6/($B$21*0.000001*K6*$B$26*$B$18))</f>
         <v>3.617225338450595</v>
       </c>
-      <c r="N6" s="79"/>
-      <c r="O6" s="2"/>
+      <c r="N6" s="115">
+        <f t="shared" si="5"/>
+        <v>119550.38210475269</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="6"/>
+        <v>8.1871449168719052E-2</v>
+      </c>
       <c r="P6" s="22"/>
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="55">
+      <c r="A7" s="54">
         <v>22</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="41" t="s">
         <v>217</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="42">
         <v>26.732850185718199</v>
       </c>
-      <c r="E7" s="63">
+      <c r="E7" s="62">
         <v>39.711930712395898</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="42">
         <v>2.6359343916865301</v>
       </c>
-      <c r="G7" s="63">
+      <c r="G7" s="62">
         <v>0.67714190377392303</v>
       </c>
-      <c r="H7" s="43">
+      <c r="H7" s="42">
         <f t="shared" si="0"/>
         <v>0.74311124513965143</v>
       </c>
-      <c r="I7" s="66">
-        <f>(D7-(1-H7)*E7)/H7</f>
+      <c r="I7" s="65">
+        <f t="shared" si="1"/>
         <v>22.24606592893597</v>
       </c>
-      <c r="J7" s="44">
-        <f t="shared" si="1"/>
+      <c r="J7" s="43">
+        <f t="shared" si="3"/>
         <v>23.182238277439122</v>
       </c>
-      <c r="K7" s="102">
+      <c r="K7" s="100">
+        <f t="shared" si="4"/>
+        <v>231.82238277439123</v>
+      </c>
+      <c r="L7" s="100">
+        <f t="shared" si="7"/>
+        <v>0.75204266710473999</v>
+      </c>
+      <c r="M7" s="100">
         <f t="shared" si="2"/>
-        <v>231.82238277439123</v>
-      </c>
-      <c r="L7" s="102">
-        <f t="shared" si="3"/>
-        <v>0.75204266710473999</v>
-      </c>
-      <c r="M7" s="102">
-        <f>E7/(1+3*0.000000000001*E7/($B$21*0.000001*K7*$B$26*$B$18))</f>
         <v>6.4253149900318576</v>
       </c>
-      <c r="N7" s="79"/>
-      <c r="O7" s="2"/>
+      <c r="N7" s="115">
+        <f t="shared" si="5"/>
+        <v>231822.38277439121</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="6"/>
+        <v>0.56018595746572353</v>
+      </c>
       <c r="P7" s="22"/>
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="54">
+      <c r="A8" s="53">
         <v>23</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="53" t="s">
         <v>212</v>
       </c>
       <c r="D8" s="2">
         <v>16.299246804189501</v>
       </c>
-      <c r="E8" s="58">
+      <c r="E8" s="57">
         <v>53.360414862107604</v>
       </c>
       <c r="F8" s="2">
         <v>2.8931738768260402</v>
       </c>
-      <c r="G8" s="58">
+      <c r="G8" s="57">
         <v>0.72605905590735997</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="0"/>
         <v>0.74904409938061378</v>
       </c>
-      <c r="I8" s="67">
-        <f>(D8-(1-H8)*E8)/H8</f>
+      <c r="I8" s="66">
+        <f t="shared" si="1"/>
         <v>3.8824627781594567</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>22.467467871025359</v>
       </c>
-      <c r="K8" s="81">
+      <c r="K8" s="79">
+        <f t="shared" si="4"/>
+        <v>224.6746787102536</v>
+      </c>
+      <c r="L8" s="79">
+        <f t="shared" si="7"/>
+        <v>0.73272274768013212</v>
+      </c>
+      <c r="M8" s="79">
         <f t="shared" si="2"/>
-        <v>224.6746787102536</v>
-      </c>
-      <c r="L8" s="81">
-        <f t="shared" si="3"/>
-        <v>0.73272274768013212</v>
-      </c>
-      <c r="M8" s="81">
-        <f>E8/(1+3*0.000000000001*E8/($B$21*0.000001*K8*$B$26*$B$18))</f>
         <v>6.5212980121876782</v>
       </c>
-      <c r="N8" s="79"/>
-      <c r="O8" s="2"/>
+      <c r="N8" s="115">
+        <f t="shared" si="5"/>
+        <v>224674.67871025359</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="6"/>
+        <v>7.2759231505084843E-2</v>
+      </c>
       <c r="P8" s="22"/>
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
     </row>
     <row r="9" spans="1:18" s="25" customFormat="1">
-      <c r="A9" s="55">
+      <c r="A9" s="54">
         <v>35</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="41" t="s">
         <v>265</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="42">
         <v>5.8842396681164404</v>
       </c>
-      <c r="E9" s="63">
+      <c r="E9" s="62">
         <v>34.9883130236109</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="42">
         <v>2.7798993676274999</v>
       </c>
-      <c r="G9" s="63">
+      <c r="G9" s="62">
         <v>0.56505400079923995</v>
       </c>
-      <c r="H9" s="43">
+      <c r="H9" s="42">
         <f t="shared" si="0"/>
         <v>0.79673580728158366</v>
       </c>
-      <c r="I9" s="66">
-        <f>(D9-(1-H9)*E9)/H9</f>
+      <c r="I9" s="65">
+        <f t="shared" si="1"/>
         <v>-1.540826359236557</v>
       </c>
-      <c r="J9" s="44">
-        <f t="shared" si="1"/>
+      <c r="J9" s="43">
+        <f t="shared" si="3"/>
         <v>17.108449358859719</v>
       </c>
-      <c r="K9" s="102">
+      <c r="K9" s="100">
+        <f t="shared" si="4"/>
+        <v>171.08449358859718</v>
+      </c>
+      <c r="L9" s="100">
+        <f t="shared" si="7"/>
+        <v>0.556717925663758</v>
+      </c>
+      <c r="M9" s="100">
         <f t="shared" si="2"/>
-        <v>171.08449358859718</v>
-      </c>
-      <c r="L9" s="102">
-        <f t="shared" si="3"/>
-        <v>0.556717925663758</v>
-      </c>
-      <c r="M9" s="102">
-        <f>E9/(1+3*0.000000000001*E9/($B$21*0.000001*K9*$B$26*$B$18))</f>
         <v>4.8698044785830383</v>
       </c>
-      <c r="N9" s="79"/>
-      <c r="O9" s="2"/>
+      <c r="N9" s="115">
+        <f t="shared" si="5"/>
+        <v>171084.49358859716</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="6"/>
+        <v>-4.4038315256776532E-2</v>
+      </c>
       <c r="P9" s="22"/>
       <c r="Q9" s="22"/>
       <c r="R9" s="22"/>
     </row>
     <row r="10" spans="1:18" s="25" customFormat="1">
-      <c r="A10" s="88"/>
-      <c r="B10" s="89"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="91"/>
-      <c r="F10" s="90"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="90"/>
-      <c r="K10" s="93"/>
-      <c r="L10" s="93"/>
-      <c r="M10" s="91"/>
-      <c r="N10" s="80"/>
+      <c r="A10" s="86"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="91"/>
+      <c r="M10" s="89"/>
+      <c r="N10" s="78"/>
       <c r="O10" s="21"/>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="55" t="s">
         <v>242</v>
       </c>
       <c r="B11" s="39"/>
-      <c r="C11" s="56"/>
+      <c r="C11" s="55"/>
       <c r="D11" s="26">
-        <f t="shared" ref="D11:K11" si="4">AVERAGE(D3:D9)</f>
+        <f t="shared" ref="D11:K11" si="8">AVERAGE(D3:D9)</f>
         <v>12.822428494224852</v>
       </c>
-      <c r="E11" s="59">
-        <f t="shared" si="4"/>
+      <c r="E11" s="58">
+        <f t="shared" si="8"/>
         <v>41.326320771271405</v>
       </c>
       <c r="F11" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3.1442735107485187</v>
       </c>
-      <c r="G11" s="59">
-        <f t="shared" si="4"/>
+      <c r="G11" s="58">
+        <f t="shared" si="8"/>
         <v>0.64222142154123518</v>
       </c>
       <c r="H11" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.79035511101129763</v>
       </c>
-      <c r="I11" s="59">
-        <f t="shared" si="4"/>
+      <c r="I11" s="58">
+        <f t="shared" si="8"/>
         <v>5.2242409632684588</v>
       </c>
       <c r="J11" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>17.998674160848768</v>
       </c>
-      <c r="K11" s="82">
-        <f t="shared" si="4"/>
+      <c r="K11" s="80">
+        <f t="shared" si="8"/>
         <v>179.98674160848765</v>
       </c>
-      <c r="L11" s="82">
-        <f t="shared" ref="L11:M11" si="5">AVERAGE(L3:L9)</f>
+      <c r="L11" s="80">
+        <f t="shared" ref="L11:M11" si="9">AVERAGE(L3:L9)</f>
         <v>0.58638685255224055</v>
       </c>
-      <c r="M11" s="82">
-        <f t="shared" si="5"/>
+      <c r="M11" s="80">
+        <f t="shared" si="9"/>
         <v>5.1799495411236292</v>
       </c>
-      <c r="N11" s="79"/>
-      <c r="O11" s="2"/>
+      <c r="N11" s="116">
+        <f t="shared" ref="N11:O11" si="10">AVERAGE(N3:N9)</f>
+        <v>179986.74160848765</v>
+      </c>
+      <c r="O11" s="120">
+        <f t="shared" si="10"/>
+        <v>0.12906069277200327</v>
+      </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="53" t="s">
         <v>241</v>
       </c>
       <c r="B12" s="19"/>
-      <c r="C12" s="54"/>
+      <c r="C12" s="53"/>
       <c r="D12" s="2">
-        <f t="shared" ref="D12:K12" si="6">STDEVA(D3:D9)</f>
+        <f t="shared" ref="D12:K12" si="11">STDEVA(D3:D9)</f>
         <v>6.9731889016687632</v>
       </c>
-      <c r="E12" s="58">
-        <f t="shared" si="6"/>
+      <c r="E12" s="57">
+        <f t="shared" si="11"/>
         <v>7.2057868063392618</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.60343176745670168</v>
       </c>
-      <c r="G12" s="58">
-        <f t="shared" si="6"/>
+      <c r="G12" s="57">
+        <f t="shared" si="11"/>
         <v>7.9487171526184133E-2</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4.2877750625749327E-2</v>
       </c>
-      <c r="I12" s="67">
+      <c r="I12" s="66">
         <f>STDEVA(I3:I9)</f>
         <v>7.827543083818524</v>
       </c>
       <c r="J12" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4.5343429914199413</v>
       </c>
-      <c r="K12" s="86">
-        <f t="shared" si="6"/>
+      <c r="K12" s="84">
+        <f t="shared" si="11"/>
         <v>45.343429914199454</v>
       </c>
-      <c r="L12" s="86">
-        <f t="shared" ref="L12:M12" si="7">STDEVA(L3:L9)</f>
+      <c r="L12" s="84">
+        <f t="shared" ref="L12:M12" si="12">STDEVA(L3:L9)</f>
         <v>0.14659136279613694</v>
       </c>
-      <c r="M12" s="86">
-        <f t="shared" si="7"/>
+      <c r="M12" s="84">
+        <f t="shared" si="12"/>
         <v>1.2190560903217424</v>
       </c>
-      <c r="N12" s="81"/>
-      <c r="O12" s="2"/>
+      <c r="N12" s="117">
+        <f t="shared" ref="N12:O12" si="13">STDEVA(N3:N9)</f>
+        <v>45343.429914199492</v>
+      </c>
+      <c r="O12" s="121">
+        <f t="shared" si="13"/>
+        <v>0.1991764635079134</v>
+      </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="56" t="s">
+      <c r="A13" s="55" t="s">
         <v>240</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="56"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="55"/>
       <c r="D13" s="28">
-        <f t="shared" ref="D13:K13" si="8">D12/SQRT(COUNT(D3:D9)-1)</f>
+        <f t="shared" ref="D13:K13" si="14">D12/SQRT(COUNT(D3:D9)-1)</f>
         <v>2.8467924481878555</v>
       </c>
-      <c r="E13" s="59">
-        <f t="shared" si="8"/>
+      <c r="E13" s="58">
+        <f t="shared" si="14"/>
         <v>2.9417501451350629</v>
       </c>
       <c r="F13" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.24634998747578582</v>
       </c>
-      <c r="G13" s="59">
-        <f t="shared" si="8"/>
+      <c r="G13" s="58">
+        <f t="shared" si="14"/>
         <v>3.2450501889372527E-2</v>
       </c>
       <c r="H13" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.7504768391897997E-2</v>
       </c>
-      <c r="I13" s="59">
-        <f t="shared" si="8"/>
+      <c r="I13" s="58">
+        <f t="shared" si="14"/>
         <v>3.195581082501147</v>
       </c>
       <c r="J13" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.8511377746239899</v>
       </c>
-      <c r="K13" s="82">
-        <f t="shared" si="8"/>
+      <c r="K13" s="80">
+        <f t="shared" si="14"/>
         <v>18.511377746239916</v>
       </c>
-      <c r="L13" s="82">
-        <f t="shared" ref="L13:M13" si="9">L12/SQRT(COUNT(L3:L9)-1)</f>
+      <c r="L13" s="80">
+        <f t="shared" ref="L13:M13" si="15">L12/SQRT(COUNT(L3:L9)-1)</f>
         <v>5.9845673258290842E-2</v>
       </c>
-      <c r="M13" s="82">
-        <f t="shared" si="9"/>
+      <c r="M13" s="80">
+        <f t="shared" si="15"/>
         <v>0.49767756485341197</v>
       </c>
-      <c r="N13" s="81"/>
+      <c r="N13" s="116">
+        <f t="shared" ref="N13:O13" si="16">N12/SQRT(COUNT(N3:N9)-1)</f>
+        <v>18511.37774623993</v>
+      </c>
+      <c r="O13" s="120">
+        <f t="shared" si="16"/>
+        <v>8.1313450727743652E-2</v>
+      </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
@@ -9918,146 +10113,146 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9BB0BB4-F947-9945-841E-63ED0AB16818}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="29" style="110" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" style="108" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="113" t="s">
         <v>309</v>
       </c>
-      <c r="B1" s="116" t="s">
+      <c r="B1" s="114" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="109" t="s">
         <v>294</v>
       </c>
-      <c r="B2" s="70">
+      <c r="B2" s="69">
         <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="109" t="s">
         <v>295</v>
       </c>
-      <c r="B3" s="70">
+      <c r="B3" s="69">
         <f>2*124</f>
         <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="111" t="s">
+      <c r="A4" s="109" t="s">
         <v>296</v>
       </c>
-      <c r="B4" s="112">
+      <c r="B4" s="110">
         <v>4.0000000000000001E-10</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="113" t="s">
+      <c r="A5" s="111" t="s">
         <v>297</v>
       </c>
-      <c r="B5" s="112">
+      <c r="B5" s="110">
         <f>B2*B4</f>
         <v>4.9600000000000001E-8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="113" t="s">
+      <c r="A6" s="111" t="s">
         <v>298</v>
       </c>
-      <c r="B6" s="112">
+      <c r="B6" s="110">
         <f>B3*B4</f>
         <v>9.9200000000000002E-8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="111" t="s">
+      <c r="A7" s="109" t="s">
         <v>299</v>
       </c>
-      <c r="B7" s="112">
+      <c r="B7" s="110">
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="111" t="s">
+      <c r="A8" s="109" t="s">
         <v>300</v>
       </c>
-      <c r="B8" s="112">
+      <c r="B8" s="110">
         <v>1000000000</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="34">
-      <c r="A9" s="114" t="s">
+      <c r="A9" s="112" t="s">
         <v>302</v>
       </c>
-      <c r="B9" s="70">
+      <c r="B9" s="69">
         <v>0.8</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="34">
-      <c r="A10" s="114" t="s">
+      <c r="A10" s="112" t="s">
         <v>308</v>
       </c>
-      <c r="B10" s="70">
+      <c r="B10" s="69">
         <f>B9/14912</f>
         <v>5.3648068669527901E-5</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="34">
-      <c r="A11" s="114" t="s">
+      <c r="A11" s="112" t="s">
         <v>303</v>
       </c>
-      <c r="B11" s="70">
+      <c r="B11" s="69">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="34">
-      <c r="A12" s="114" t="s">
+      <c r="A12" s="112" t="s">
         <v>307</v>
       </c>
-      <c r="B12" s="70">
+      <c r="B12" s="69">
         <f>B11/14912</f>
         <v>6.7060085836909871E-4</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="34">
-      <c r="A13" s="114" t="s">
+      <c r="A13" s="112" t="s">
         <v>301</v>
       </c>
-      <c r="B13" s="70">
+      <c r="B13" s="69">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="34">
-      <c r="A14" s="114" t="s">
+      <c r="A14" s="112" t="s">
         <v>305</v>
       </c>
-      <c r="B14" s="70">
+      <c r="B14" s="69">
         <f>B13/(2*14912)</f>
         <v>6.7060085836909871E-5</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="34">
-      <c r="A15" s="114" t="s">
+      <c r="A15" s="112" t="s">
         <v>304</v>
       </c>
-      <c r="B15" s="70">
+      <c r="B15" s="69">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="34">
-      <c r="A16" s="114" t="s">
+      <c r="A16" s="112" t="s">
         <v>306</v>
       </c>
-      <c r="B16" s="70">
+      <c r="B16" s="69">
         <f>B15/(2*14912)</f>
         <v>6.7060085836909871E-4</v>
       </c>

</xml_diff>